<commit_message>
Continue Add Menu Production Warehouse
</commit_message>
<xml_diff>
--- a/List Menu.xlsx
+++ b/List Menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\onlineguide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4361D6-A160-4B56-ADD4-1BF1A878DC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1252E60-4C0C-40DB-B4CE-63555F8B594A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{40BDCF54-5589-495D-8190-883E443269E3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="124">
   <si>
     <t>Menu</t>
   </si>
@@ -308,9 +308,6 @@
     <t>Purchase and Exchange (Exchange)</t>
   </si>
   <si>
-    <t>purchas_and_exchange</t>
-  </si>
-  <si>
     <t>Purchasing and Exchange Records</t>
   </si>
   <si>
@@ -351,6 +348,66 @@
   </si>
   <si>
     <t>purchased_optical_fiberdata</t>
+  </si>
+  <si>
+    <t>purchase_and_exchange</t>
+  </si>
+  <si>
+    <t>Production Warehousing</t>
+  </si>
+  <si>
+    <t>production_warehousing</t>
+  </si>
+  <si>
+    <t>Production Input Record</t>
+  </si>
+  <si>
+    <t>production_input_record</t>
+  </si>
+  <si>
+    <t>Printing of Production Input Documents</t>
+  </si>
+  <si>
+    <t>printing_of_production_input_documents</t>
+  </si>
+  <si>
+    <t>Production Order Record</t>
+  </si>
+  <si>
+    <t>production_order_record</t>
+  </si>
+  <si>
+    <t>Production Warehousing Record Details</t>
+  </si>
+  <si>
+    <t>production_warehousing_record_details</t>
+  </si>
+  <si>
+    <t>Collect Material Out of Warehouse</t>
+  </si>
+  <si>
+    <t>Material Requisition - MES Production Order</t>
+  </si>
+  <si>
+    <t>material_requisition</t>
+  </si>
+  <si>
+    <t>Material Return Application - MES Production Order</t>
+  </si>
+  <si>
+    <t>material_return_application</t>
+  </si>
+  <si>
+    <t>Material Request - Cost Center</t>
+  </si>
+  <si>
+    <t>material_request</t>
+  </si>
+  <si>
+    <t>Return Application - Cost Center</t>
+  </si>
+  <si>
+    <t>return_application</t>
   </si>
 </sst>
 </file>
@@ -374,15 +431,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -429,31 +492,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -791,14 +871,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46758F73-D68C-4007-AE73-B5A0F2E8918A}">
   <dimension ref="A1:C150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.453125" customWidth="1"/>
-    <col min="2" max="2" width="34.1796875" customWidth="1"/>
+    <col min="2" max="2" width="42.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.26953125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -814,958 +894,1000 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="5"/>
+      <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="5"/>
+      <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="5"/>
+      <c r="B14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="5"/>
+      <c r="B15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="5"/>
+      <c r="B17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="5"/>
+      <c r="B18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3" t="s">
+      <c r="A19" s="5"/>
+      <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3" t="s">
+      <c r="A20" s="5"/>
+      <c r="B20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3" t="s">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3" t="s">
+      <c r="A22" s="5"/>
+      <c r="B22" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3" t="s">
+      <c r="A23" s="5"/>
+      <c r="B23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2"/>
-      <c r="B24" s="3" t="s">
+      <c r="A24" s="5"/>
+      <c r="B24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-      <c r="B25" s="3" t="s">
+      <c r="A25" s="5"/>
+      <c r="B25" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-      <c r="B26" s="3" t="s">
+      <c r="A26" s="5"/>
+      <c r="B26" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-      <c r="B27" s="3" t="s">
+      <c r="A27" s="5"/>
+      <c r="B27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
-      <c r="B28" s="3" t="s">
+      <c r="A28" s="5"/>
+      <c r="B28" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
-      <c r="B29" s="3" t="s">
+      <c r="A29" s="5"/>
+      <c r="B29" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
-      <c r="B30" s="3" t="s">
+      <c r="A30" s="5"/>
+      <c r="B30" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
-      <c r="B31" s="3" t="s">
+      <c r="A31" s="5"/>
+      <c r="B31" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-      <c r="B32" s="3" t="s">
+      <c r="A32" s="5"/>
+      <c r="B32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-      <c r="B33" s="3" t="s">
+      <c r="A33" s="5"/>
+      <c r="B33" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="5"/>
-      <c r="B35" s="3" t="s">
+      <c r="A35" s="7"/>
+      <c r="B35" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="4" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="5"/>
-      <c r="B36" s="3" t="s">
+      <c r="A36" s="7"/>
+      <c r="B36" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="5"/>
-      <c r="B37" s="3" t="s">
+      <c r="A37" s="7"/>
+      <c r="B37" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="4" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="5"/>
-      <c r="B38" s="3" t="s">
+      <c r="A38" s="7"/>
+      <c r="B38" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="4" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="5"/>
-      <c r="B39" s="6" t="s">
+      <c r="A39" s="7"/>
+      <c r="B39" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="4" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="5"/>
-      <c r="B40" s="3" t="s">
+      <c r="A40" s="7"/>
+      <c r="B40" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="5"/>
-      <c r="B41" s="3" t="s">
+      <c r="A41" s="7"/>
+      <c r="B41" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="5"/>
-      <c r="B42" s="3" t="s">
+      <c r="A42" s="7"/>
+      <c r="B42" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="5"/>
-      <c r="B43" s="3" t="s">
+      <c r="A43" s="7"/>
+      <c r="B43" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="4" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="5"/>
-      <c r="B44" s="3" t="s">
+      <c r="A44" s="7"/>
+      <c r="B44" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="7"/>
+      <c r="B45" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="5"/>
-      <c r="B45" s="3" t="s">
+      <c r="C45" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C45" s="3" t="s">
+    </row>
+    <row r="46" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="7"/>
+      <c r="B46" s="8" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="5"/>
-      <c r="B46" s="6" t="s">
+      <c r="C46" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="3" t="s">
+    </row>
+    <row r="47" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="7"/>
+      <c r="B47" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="5"/>
-      <c r="B47" s="6" t="s">
+      <c r="C47" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C47" s="3" t="s">
+    </row>
+    <row r="48" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="7"/>
+      <c r="B48" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="5"/>
-      <c r="B48" s="3" t="s">
+      <c r="C48" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C48" s="3" t="s">
+    </row>
+    <row r="49" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="7"/>
+      <c r="B49" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="5"/>
-      <c r="B49" s="3" t="s">
+      <c r="C49" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C49" s="3" t="s">
+    </row>
+    <row r="50" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="7"/>
+      <c r="B50" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="5"/>
-      <c r="B50" s="3" t="s">
+      <c r="C50" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="3" t="s">
+    </row>
+    <row r="51" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="7"/>
+      <c r="B51" s="9" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="5"/>
-      <c r="B51" s="7" t="s">
+      <c r="C51" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C51" s="7" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="52" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="8"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
+      <c r="A52" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="53" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="8"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
+      <c r="A53" s="7"/>
+      <c r="B53" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="54" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="8"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
+      <c r="A54" s="7"/>
+      <c r="B54" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="55" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="8"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
+      <c r="A55" s="7"/>
+      <c r="B55" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="56" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="8"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
+      <c r="A56" s="10"/>
+      <c r="B56" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="57" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="8"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
+      <c r="A57" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="58" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="8"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
+      <c r="A58" s="7"/>
+      <c r="B58" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="59" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="8"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
+      <c r="A59" s="7"/>
+      <c r="B59" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="60" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="8"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
+      <c r="A60" s="7"/>
+      <c r="B60" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="61" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="8"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
+      <c r="A61" s="7"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
     </row>
     <row r="62" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="8"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
+      <c r="A62" s="7"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
     </row>
     <row r="63" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="8"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
+      <c r="A63" s="7"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
     </row>
     <row r="64" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="8"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
+      <c r="A64" s="7"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
     </row>
     <row r="65" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="8"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
+      <c r="A65" s="7"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
     </row>
     <row r="66" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="8"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
+      <c r="A66" s="7"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
     </row>
     <row r="67" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="8"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
+      <c r="A67" s="7"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
     </row>
     <row r="68" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="8"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
+      <c r="A68" s="7"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
     </row>
     <row r="69" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="8"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
+      <c r="A69" s="7"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
     </row>
     <row r="70" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="8"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
+      <c r="A70" s="7"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
     </row>
     <row r="71" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="8"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
+      <c r="A71" s="7"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
     </row>
     <row r="72" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="8"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
+      <c r="A72" s="10"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
     </row>
     <row r="73" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="8"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
+      <c r="A73" s="3"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
     </row>
     <row r="74" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="8"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
+      <c r="A74" s="3"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
     </row>
     <row r="75" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="8"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
+      <c r="A75" s="3"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
     </row>
     <row r="76" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="8"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
+      <c r="A76" s="3"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
     </row>
     <row r="77" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="8"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
+      <c r="A77" s="3"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
     </row>
     <row r="78" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="8"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
+      <c r="A78" s="3"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
     </row>
     <row r="79" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="8"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
+      <c r="A79" s="3"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
     </row>
     <row r="80" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="8"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
+      <c r="A80" s="3"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
     </row>
     <row r="81" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="8"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
+      <c r="A81" s="3"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
     </row>
     <row r="82" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="8"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
+      <c r="A82" s="3"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
     </row>
     <row r="83" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="8"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
+      <c r="A83" s="3"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
     </row>
     <row r="84" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="8"/>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
+      <c r="A84" s="3"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
     </row>
     <row r="85" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="8"/>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
+      <c r="A85" s="3"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
     </row>
     <row r="86" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="8"/>
-      <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
+      <c r="A86" s="3"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
     </row>
     <row r="87" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="8"/>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
+      <c r="A87" s="3"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
     </row>
     <row r="88" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="8"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
+      <c r="A88" s="3"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
     </row>
     <row r="89" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="8"/>
-      <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
+      <c r="A89" s="3"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
     </row>
     <row r="90" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="8"/>
-      <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
+      <c r="A90" s="3"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
     </row>
     <row r="91" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="8"/>
-      <c r="B91" s="3"/>
-      <c r="C91" s="3"/>
+      <c r="A91" s="3"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
     </row>
     <row r="92" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="8"/>
-      <c r="B92" s="3"/>
-      <c r="C92" s="3"/>
+      <c r="A92" s="3"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
     </row>
     <row r="93" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="8"/>
-      <c r="B93" s="3"/>
-      <c r="C93" s="3"/>
+      <c r="A93" s="3"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
     </row>
     <row r="94" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="8"/>
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
+      <c r="A94" s="3"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
     </row>
     <row r="95" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="8"/>
-      <c r="B95" s="3"/>
-      <c r="C95" s="3"/>
+      <c r="A95" s="3"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
     </row>
     <row r="96" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="8"/>
-      <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
+      <c r="A96" s="3"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
     </row>
     <row r="97" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="8"/>
-      <c r="B97" s="3"/>
-      <c r="C97" s="3"/>
+      <c r="A97" s="3"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
     </row>
     <row r="98" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="8"/>
-      <c r="B98" s="3"/>
-      <c r="C98" s="3"/>
+      <c r="A98" s="3"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
     </row>
     <row r="99" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="8"/>
-      <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
+      <c r="A99" s="3"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
     </row>
     <row r="100" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="8"/>
-      <c r="B100" s="3"/>
-      <c r="C100" s="3"/>
+      <c r="A100" s="3"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
     </row>
     <row r="101" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="8"/>
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
+      <c r="A101" s="3"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
     </row>
     <row r="102" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="8"/>
-      <c r="B102" s="3"/>
-      <c r="C102" s="3"/>
+      <c r="A102" s="3"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
     </row>
     <row r="103" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="8"/>
-      <c r="B103" s="3"/>
-      <c r="C103" s="3"/>
+      <c r="A103" s="3"/>
+      <c r="B103" s="2"/>
+      <c r="C103" s="2"/>
     </row>
     <row r="104" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="8"/>
-      <c r="B104" s="3"/>
-      <c r="C104" s="3"/>
+      <c r="A104" s="3"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
     </row>
     <row r="105" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="8"/>
-      <c r="B105" s="3"/>
-      <c r="C105" s="3"/>
+      <c r="A105" s="3"/>
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
     </row>
     <row r="106" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="8"/>
-      <c r="B106" s="3"/>
-      <c r="C106" s="3"/>
+      <c r="A106" s="3"/>
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
     </row>
     <row r="107" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="8"/>
-      <c r="B107" s="3"/>
-      <c r="C107" s="3"/>
+      <c r="A107" s="3"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
     </row>
     <row r="108" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="8"/>
-      <c r="B108" s="3"/>
-      <c r="C108" s="3"/>
+      <c r="A108" s="3"/>
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
     </row>
     <row r="109" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="3"/>
-      <c r="B109" s="3"/>
-      <c r="C109" s="3"/>
+      <c r="A109" s="2"/>
+      <c r="B109" s="2"/>
+      <c r="C109" s="2"/>
     </row>
     <row r="110" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="3"/>
-      <c r="B110" s="3"/>
-      <c r="C110" s="3"/>
+      <c r="A110" s="2"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
     </row>
     <row r="111" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="3"/>
-      <c r="B111" s="3"/>
-      <c r="C111" s="3"/>
+      <c r="A111" s="2"/>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2"/>
     </row>
     <row r="112" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="3"/>
-      <c r="B112" s="3"/>
-      <c r="C112" s="3"/>
+      <c r="A112" s="2"/>
+      <c r="B112" s="2"/>
+      <c r="C112" s="2"/>
     </row>
     <row r="113" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="3"/>
-      <c r="B113" s="3"/>
-      <c r="C113" s="3"/>
+      <c r="A113" s="2"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="2"/>
     </row>
     <row r="114" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="3"/>
-      <c r="B114" s="3"/>
-      <c r="C114" s="3"/>
+      <c r="A114" s="2"/>
+      <c r="B114" s="2"/>
+      <c r="C114" s="2"/>
     </row>
     <row r="115" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="3"/>
-      <c r="B115" s="3"/>
-      <c r="C115" s="3"/>
+      <c r="A115" s="2"/>
+      <c r="B115" s="2"/>
+      <c r="C115" s="2"/>
     </row>
     <row r="116" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="3"/>
-      <c r="B116" s="3"/>
-      <c r="C116" s="3"/>
+      <c r="A116" s="2"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="2"/>
     </row>
     <row r="117" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="3"/>
-      <c r="B117" s="3"/>
-      <c r="C117" s="3"/>
+      <c r="A117" s="2"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="2"/>
     </row>
     <row r="118" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="3"/>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
+      <c r="A118" s="2"/>
+      <c r="B118" s="2"/>
+      <c r="C118" s="2"/>
     </row>
     <row r="119" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="3"/>
-      <c r="B119" s="3"/>
-      <c r="C119" s="3"/>
+      <c r="A119" s="2"/>
+      <c r="B119" s="2"/>
+      <c r="C119" s="2"/>
     </row>
     <row r="120" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="3"/>
-      <c r="B120" s="3"/>
-      <c r="C120" s="3"/>
+      <c r="A120" s="2"/>
+      <c r="B120" s="2"/>
+      <c r="C120" s="2"/>
     </row>
     <row r="121" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="3"/>
-      <c r="B121" s="3"/>
-      <c r="C121" s="3"/>
+      <c r="A121" s="2"/>
+      <c r="B121" s="2"/>
+      <c r="C121" s="2"/>
     </row>
     <row r="122" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="3"/>
-      <c r="B122" s="3"/>
-      <c r="C122" s="3"/>
+      <c r="A122" s="2"/>
+      <c r="B122" s="2"/>
+      <c r="C122" s="2"/>
     </row>
     <row r="123" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="3"/>
-      <c r="B123" s="3"/>
-      <c r="C123" s="3"/>
+      <c r="A123" s="2"/>
+      <c r="B123" s="2"/>
+      <c r="C123" s="2"/>
     </row>
     <row r="124" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="3"/>
-      <c r="B124" s="3"/>
-      <c r="C124" s="3"/>
+      <c r="A124" s="2"/>
+      <c r="B124" s="2"/>
+      <c r="C124" s="2"/>
     </row>
     <row r="125" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="3"/>
-      <c r="B125" s="3"/>
-      <c r="C125" s="3"/>
+      <c r="A125" s="2"/>
+      <c r="B125" s="2"/>
+      <c r="C125" s="2"/>
     </row>
     <row r="126" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="3"/>
-      <c r="B126" s="3"/>
-      <c r="C126" s="3"/>
+      <c r="A126" s="2"/>
+      <c r="B126" s="2"/>
+      <c r="C126" s="2"/>
     </row>
     <row r="127" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A127" s="3"/>
-      <c r="B127" s="3"/>
-      <c r="C127" s="3"/>
+      <c r="A127" s="2"/>
+      <c r="B127" s="2"/>
+      <c r="C127" s="2"/>
     </row>
     <row r="128" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="3"/>
-      <c r="B128" s="3"/>
-      <c r="C128" s="3"/>
+      <c r="A128" s="2"/>
+      <c r="B128" s="2"/>
+      <c r="C128" s="2"/>
     </row>
     <row r="129" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="3"/>
-      <c r="B129" s="3"/>
-      <c r="C129" s="3"/>
+      <c r="A129" s="2"/>
+      <c r="B129" s="2"/>
+      <c r="C129" s="2"/>
     </row>
     <row r="130" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="3"/>
-      <c r="B130" s="3"/>
-      <c r="C130" s="3"/>
+      <c r="A130" s="2"/>
+      <c r="B130" s="2"/>
+      <c r="C130" s="2"/>
     </row>
     <row r="131" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="3"/>
-      <c r="B131" s="3"/>
-      <c r="C131" s="3"/>
+      <c r="A131" s="2"/>
+      <c r="B131" s="2"/>
+      <c r="C131" s="2"/>
     </row>
     <row r="132" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A132" s="3"/>
-      <c r="B132" s="3"/>
-      <c r="C132" s="3"/>
+      <c r="A132" s="2"/>
+      <c r="B132" s="2"/>
+      <c r="C132" s="2"/>
     </row>
     <row r="133" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="3"/>
-      <c r="B133" s="3"/>
-      <c r="C133" s="3"/>
+      <c r="A133" s="2"/>
+      <c r="B133" s="2"/>
+      <c r="C133" s="2"/>
     </row>
     <row r="134" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="3"/>
-      <c r="B134" s="3"/>
-      <c r="C134" s="3"/>
+      <c r="A134" s="2"/>
+      <c r="B134" s="2"/>
+      <c r="C134" s="2"/>
     </row>
     <row r="135" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="3"/>
-      <c r="B135" s="3"/>
-      <c r="C135" s="3"/>
+      <c r="A135" s="2"/>
+      <c r="B135" s="2"/>
+      <c r="C135" s="2"/>
     </row>
     <row r="136" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="3"/>
-      <c r="B136" s="3"/>
-      <c r="C136" s="3"/>
+      <c r="A136" s="2"/>
+      <c r="B136" s="2"/>
+      <c r="C136" s="2"/>
     </row>
     <row r="137" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="3"/>
-      <c r="B137" s="3"/>
-      <c r="C137" s="3"/>
+      <c r="A137" s="2"/>
+      <c r="B137" s="2"/>
+      <c r="C137" s="2"/>
     </row>
     <row r="138" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="3"/>
-      <c r="B138" s="3"/>
-      <c r="C138" s="3"/>
+      <c r="A138" s="2"/>
+      <c r="B138" s="2"/>
+      <c r="C138" s="2"/>
     </row>
     <row r="139" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="3"/>
-      <c r="B139" s="3"/>
-      <c r="C139" s="3"/>
+      <c r="A139" s="2"/>
+      <c r="B139" s="2"/>
+      <c r="C139" s="2"/>
     </row>
     <row r="140" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="3"/>
-      <c r="B140" s="3"/>
-      <c r="C140" s="3"/>
+      <c r="A140" s="2"/>
+      <c r="B140" s="2"/>
+      <c r="C140" s="2"/>
     </row>
     <row r="141" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="3"/>
-      <c r="B141" s="3"/>
-      <c r="C141" s="3"/>
+      <c r="A141" s="2"/>
+      <c r="B141" s="2"/>
+      <c r="C141" s="2"/>
     </row>
     <row r="142" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="3"/>
-      <c r="B142" s="3"/>
-      <c r="C142" s="3"/>
+      <c r="A142" s="2"/>
+      <c r="B142" s="2"/>
+      <c r="C142" s="2"/>
     </row>
     <row r="143" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A143" s="3"/>
-      <c r="B143" s="3"/>
-      <c r="C143" s="3"/>
+      <c r="A143" s="2"/>
+      <c r="B143" s="2"/>
+      <c r="C143" s="2"/>
     </row>
     <row r="144" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="3"/>
-      <c r="B144" s="3"/>
-      <c r="C144" s="3"/>
+      <c r="A144" s="2"/>
+      <c r="B144" s="2"/>
+      <c r="C144" s="2"/>
     </row>
     <row r="145" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="3"/>
-      <c r="B145" s="3"/>
-      <c r="C145" s="3"/>
+      <c r="A145" s="2"/>
+      <c r="B145" s="2"/>
+      <c r="C145" s="2"/>
     </row>
     <row r="146" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="3"/>
-      <c r="B146" s="3"/>
-      <c r="C146" s="3"/>
+      <c r="A146" s="2"/>
+      <c r="B146" s="2"/>
+      <c r="C146" s="2"/>
     </row>
     <row r="147" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="3"/>
-      <c r="B147" s="3"/>
-      <c r="C147" s="3"/>
+      <c r="A147" s="2"/>
+      <c r="B147" s="2"/>
+      <c r="C147" s="2"/>
     </row>
     <row r="148" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A148" s="3"/>
-      <c r="B148" s="3"/>
-      <c r="C148" s="3"/>
+      <c r="A148" s="2"/>
+      <c r="B148" s="2"/>
+      <c r="C148" s="2"/>
     </row>
     <row r="149" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A149" s="3"/>
-      <c r="B149" s="3"/>
-      <c r="C149" s="3"/>
+      <c r="A149" s="2"/>
+      <c r="B149" s="2"/>
+      <c r="C149" s="2"/>
     </row>
     <row r="150" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A150" s="3"/>
-      <c r="B150" s="3"/>
-      <c r="C150" s="3"/>
+      <c r="A150" s="2"/>
+      <c r="B150" s="2"/>
+      <c r="C150" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="A34:A51"/>
+    <mergeCell ref="A52:A56"/>
+    <mergeCell ref="A57:A72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Finish create collect material out of warehouse
</commit_message>
<xml_diff>
--- a/List Menu.xlsx
+++ b/List Menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\onlineguide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1252E60-4C0C-40DB-B4CE-63555F8B594A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2188CF-C189-4DE4-9B60-B36FF42857DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{40BDCF54-5589-495D-8190-883E443269E3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="204">
   <si>
     <t>Menu</t>
   </si>
@@ -389,25 +389,265 @@
     <t>Material Requisition - MES Production Order</t>
   </si>
   <si>
-    <t>material_requisition</t>
-  </si>
-  <si>
     <t>Material Return Application - MES Production Order</t>
   </si>
   <si>
-    <t>material_return_application</t>
-  </si>
-  <si>
     <t>Material Request - Cost Center</t>
   </si>
   <si>
-    <t>material_request</t>
-  </si>
-  <si>
     <t>Return Application - Cost Center</t>
   </si>
   <si>
-    <t>return_application</t>
+    <t>Claim Application - Internal Order</t>
+  </si>
+  <si>
+    <t>Return Application - Internal Order</t>
+  </si>
+  <si>
+    <t>return_application_cost_center</t>
+  </si>
+  <si>
+    <t>claim_application_internal_order</t>
+  </si>
+  <si>
+    <t>return_application_internal_order</t>
+  </si>
+  <si>
+    <t>Material Request - Supplier</t>
+  </si>
+  <si>
+    <t>material_request_cost_center</t>
+  </si>
+  <si>
+    <t>material_request_supplier</t>
+  </si>
+  <si>
+    <t>Return Application - Supplier</t>
+  </si>
+  <si>
+    <t>return_application_supplier</t>
+  </si>
+  <si>
+    <t>Material Request - Line Side Warehouse</t>
+  </si>
+  <si>
+    <t>Return Application - Line Side Warehouse</t>
+  </si>
+  <si>
+    <t>material_request_lineside_warehouse</t>
+  </si>
+  <si>
+    <t>return_application_lineside_warehouse</t>
+  </si>
+  <si>
+    <t>Application for Distribution</t>
+  </si>
+  <si>
+    <t>application_for_distribution</t>
+  </si>
+  <si>
+    <t>Material Dispensing Operation</t>
+  </si>
+  <si>
+    <t>material_dispensing_operation</t>
+  </si>
+  <si>
+    <t>Material Dispensing Operation (Reinforcing Material)</t>
+  </si>
+  <si>
+    <t>material_dispensing_operation_reinforcing_material</t>
+  </si>
+  <si>
+    <t>Internal Requisition (Batch)</t>
+  </si>
+  <si>
+    <t>internal_requisition_batch</t>
+  </si>
+  <si>
+    <t>Internal Requisition (Scrap)</t>
+  </si>
+  <si>
+    <t>internal_requisition_scrap</t>
+  </si>
+  <si>
+    <t>Selling Out of Warehouse</t>
+  </si>
+  <si>
+    <t>Sales Order</t>
+  </si>
+  <si>
+    <t>sales_order</t>
+  </si>
+  <si>
+    <t>Sales Order Detail</t>
+  </si>
+  <si>
+    <t>sales_order_detail</t>
+  </si>
+  <si>
+    <t>Delivery Arrangement</t>
+  </si>
+  <si>
+    <t>delivery_arrangement</t>
+  </si>
+  <si>
+    <t>selling_out_of_warehouse</t>
+  </si>
+  <si>
+    <t>Sales Delivery Bill</t>
+  </si>
+  <si>
+    <t>sales_delivery_bill</t>
+  </si>
+  <si>
+    <t>Exit Permit</t>
+  </si>
+  <si>
+    <t>exit_permit</t>
+  </si>
+  <si>
+    <t>Checklist</t>
+  </si>
+  <si>
+    <t>checklist</t>
+  </si>
+  <si>
+    <t>Isolation Requirements</t>
+  </si>
+  <si>
+    <t>isolation_requirements</t>
+  </si>
+  <si>
+    <t>High Standard Requirement</t>
+  </si>
+  <si>
+    <t>high_standard_requirement</t>
+  </si>
+  <si>
+    <t>Maintenance of Non-standard Coefficient Length</t>
+  </si>
+  <si>
+    <t>maintenance_of_non-standard_coefficient_length</t>
+  </si>
+  <si>
+    <t>Default Picking Parameters</t>
+  </si>
+  <si>
+    <t>default_picking_parameters</t>
+  </si>
+  <si>
+    <t>Combination Characteristics</t>
+  </si>
+  <si>
+    <t>combination_characteristics</t>
+  </si>
+  <si>
+    <t>Depot Planning Arrangement</t>
+  </si>
+  <si>
+    <t>depot_planning_arrangement</t>
+  </si>
+  <si>
+    <t>Packing List Scanning Record</t>
+  </si>
+  <si>
+    <t>packing_list_scanning_record</t>
+  </si>
+  <si>
+    <t>Pre-sale Arrangement</t>
+  </si>
+  <si>
+    <t>pre-sale_arrangement</t>
+  </si>
+  <si>
+    <t>Packing List</t>
+  </si>
+  <si>
+    <t>packing_list</t>
+  </si>
+  <si>
+    <t>Sales Exit Inspection</t>
+  </si>
+  <si>
+    <t>sales_exit_inspection</t>
+  </si>
+  <si>
+    <t>Maintenance of Stock Notes</t>
+  </si>
+  <si>
+    <t>maintenance_of_stock_notes</t>
+  </si>
+  <si>
+    <t>Quality Requirements</t>
+  </si>
+  <si>
+    <t>quality_requirements</t>
+  </si>
+  <si>
+    <t>Picking Scheme</t>
+  </si>
+  <si>
+    <t>picking_scheme</t>
+  </si>
+  <si>
+    <t>Picking List</t>
+  </si>
+  <si>
+    <t>picking_list</t>
+  </si>
+  <si>
+    <t>Outbound Planning Generation</t>
+  </si>
+  <si>
+    <t>outbound_planning_generation</t>
+  </si>
+  <si>
+    <t>Delivery Requirements</t>
+  </si>
+  <si>
+    <t>delivery_requirements</t>
+  </si>
+  <si>
+    <t>Details of Packing List</t>
+  </si>
+  <si>
+    <t>details_of_packing_list</t>
+  </si>
+  <si>
+    <t>Delivery Inspection Details of Sales</t>
+  </si>
+  <si>
+    <t>delivery_inspection_details_of_sales</t>
+  </si>
+  <si>
+    <t>Outbound Planning Confirmation</t>
+  </si>
+  <si>
+    <t>outbound_planning_confirmation</t>
+  </si>
+  <si>
+    <t>Customer Group Maintenance</t>
+  </si>
+  <si>
+    <t>customer_group_maintenance</t>
+  </si>
+  <si>
+    <t>Outbound Order Management</t>
+  </si>
+  <si>
+    <t>outbound_order_management</t>
+  </si>
+  <si>
+    <t>Create Outbound Order</t>
+  </si>
+  <si>
+    <t>create_outbound_order</t>
+  </si>
+  <si>
+    <t>material_requisition_production_order</t>
+  </si>
+  <si>
+    <t>material_return_application_production_order</t>
   </si>
 </sst>
 </file>
@@ -519,6 +759,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -528,10 +772,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -871,15 +1111,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46758F73-D68C-4007-AE73-B5A0F2E8918A}">
   <dimension ref="A1:C150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.453125" customWidth="1"/>
-    <col min="2" max="2" width="42.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.26953125" customWidth="1"/>
+    <col min="2" max="2" width="43.81640625" customWidth="1"/>
+    <col min="3" max="3" width="43.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
@@ -894,10 +1134,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -905,8 +1145,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -914,277 +1154,277 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="5"/>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="5"/>
-      <c r="B16" s="2" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="5"/>
-      <c r="B17" s="2" t="s">
+      <c r="A17" s="7"/>
+      <c r="B17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="5"/>
-      <c r="B18" s="2" t="s">
+      <c r="A18" s="7"/>
+      <c r="B18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
-      <c r="B19" s="2" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="5"/>
-      <c r="B20" s="2" t="s">
+      <c r="A20" s="7"/>
+      <c r="B20" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="5"/>
-      <c r="B21" s="2" t="s">
+      <c r="A21" s="7"/>
+      <c r="B21" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="5"/>
-      <c r="B22" s="2" t="s">
+      <c r="A22" s="7"/>
+      <c r="B22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="5"/>
-      <c r="B23" s="2" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="5"/>
-      <c r="B24" s="2" t="s">
+      <c r="A24" s="7"/>
+      <c r="B24" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="5"/>
-      <c r="B25" s="2" t="s">
+      <c r="A25" s="7"/>
+      <c r="B25" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="5"/>
-      <c r="B26" s="2" t="s">
+      <c r="A26" s="7"/>
+      <c r="B26" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="5"/>
-      <c r="B27" s="2" t="s">
+      <c r="A27" s="7"/>
+      <c r="B27" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="5"/>
-      <c r="B28" s="2" t="s">
+      <c r="A28" s="7"/>
+      <c r="B28" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="5"/>
-      <c r="B29" s="2" t="s">
+      <c r="A29" s="7"/>
+      <c r="B29" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="5"/>
-      <c r="B30" s="2" t="s">
+      <c r="A30" s="7"/>
+      <c r="B30" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="5"/>
-      <c r="B31" s="2" t="s">
+      <c r="A31" s="7"/>
+      <c r="B31" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="5"/>
-      <c r="B32" s="2" t="s">
+      <c r="A32" s="7"/>
+      <c r="B32" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="5"/>
-      <c r="B33" s="2" t="s">
+      <c r="A33" s="7"/>
+      <c r="B33" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="8" t="s">
         <v>68</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -1195,7 +1435,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="7"/>
+      <c r="A35" s="9"/>
       <c r="B35" s="4" t="s">
         <v>71</v>
       </c>
@@ -1204,7 +1444,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="7"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="4" t="s">
         <v>73</v>
       </c>
@@ -1213,7 +1453,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="7"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="4" t="s">
         <v>75</v>
       </c>
@@ -1222,7 +1462,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="7"/>
+      <c r="A38" s="9"/>
       <c r="B38" s="4" t="s">
         <v>77</v>
       </c>
@@ -1231,8 +1471,8 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="7"/>
-      <c r="B39" s="8" t="s">
+      <c r="A39" s="9"/>
+      <c r="B39" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C39" s="4" t="s">
@@ -1240,7 +1480,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="7"/>
+      <c r="A40" s="9"/>
       <c r="B40" s="4" t="s">
         <v>81</v>
       </c>
@@ -1249,7 +1489,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="7"/>
+      <c r="A41" s="9"/>
       <c r="B41" s="4" t="s">
         <v>83</v>
       </c>
@@ -1258,7 +1498,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="7"/>
+      <c r="A42" s="9"/>
       <c r="B42" s="4" t="s">
         <v>85</v>
       </c>
@@ -1267,7 +1507,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="7"/>
+      <c r="A43" s="9"/>
       <c r="B43" s="4" t="s">
         <v>87</v>
       </c>
@@ -1276,7 +1516,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="7"/>
+      <c r="A44" s="9"/>
       <c r="B44" s="4" t="s">
         <v>89</v>
       </c>
@@ -1285,7 +1525,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="7"/>
+      <c r="A45" s="9"/>
       <c r="B45" s="4" t="s">
         <v>90</v>
       </c>
@@ -1294,8 +1534,8 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="7"/>
-      <c r="B46" s="8" t="s">
+      <c r="A46" s="9"/>
+      <c r="B46" s="5" t="s">
         <v>92</v>
       </c>
       <c r="C46" s="4" t="s">
@@ -1303,8 +1543,8 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="7"/>
-      <c r="B47" s="8" t="s">
+      <c r="A47" s="9"/>
+      <c r="B47" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C47" s="4" t="s">
@@ -1312,7 +1552,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="7"/>
+      <c r="A48" s="9"/>
       <c r="B48" s="4" t="s">
         <v>96</v>
       </c>
@@ -1321,7 +1561,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="7"/>
+      <c r="A49" s="9"/>
       <c r="B49" s="4" t="s">
         <v>98</v>
       </c>
@@ -1330,7 +1570,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="7"/>
+      <c r="A50" s="9"/>
       <c r="B50" s="4" t="s">
         <v>100</v>
       </c>
@@ -1339,298 +1579,460 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="7"/>
-      <c r="B51" s="9" t="s">
+      <c r="A51" s="9"/>
+      <c r="B51" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="6" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="4" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="7"/>
-      <c r="B53" s="2" t="s">
+      <c r="A53" s="9"/>
+      <c r="B53" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="4" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="7"/>
-      <c r="B54" s="2" t="s">
+      <c r="A54" s="9"/>
+      <c r="B54" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="4" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="7"/>
-      <c r="B55" s="2" t="s">
+      <c r="A55" s="9"/>
+      <c r="B55" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="4" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="10"/>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="4" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="9"/>
+      <c r="B58" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="7"/>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="9"/>
+      <c r="B59" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C59" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="9"/>
+      <c r="B60" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="7"/>
-      <c r="B59" s="2" t="s">
+      <c r="C60" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="9"/>
+      <c r="B61" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C61" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="9"/>
+      <c r="B62" s="4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="7"/>
-      <c r="B60" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="7"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-    </row>
-    <row r="62" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="7"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
+      <c r="C62" s="4" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="63" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="7"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
+      <c r="A63" s="9"/>
+      <c r="B63" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="64" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="7"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
+      <c r="A64" s="9"/>
+      <c r="B64" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="65" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="7"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
+      <c r="A65" s="9"/>
+      <c r="B65" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="66" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="7"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
+      <c r="A66" s="9"/>
+      <c r="B66" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="67" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="7"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
+      <c r="A67" s="9"/>
+      <c r="B67" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="68" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="7"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
+      <c r="A68" s="9"/>
+      <c r="B68" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="69" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="7"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
+      <c r="A69" s="9"/>
+      <c r="B69" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="70" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="7"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
+      <c r="A70" s="9"/>
+      <c r="B70" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="71" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="7"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
+      <c r="A71" s="9"/>
+      <c r="B71" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="72" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="10"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
+      <c r="A72" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="73" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="3"/>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
+      <c r="A73" s="9"/>
+      <c r="B73" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="74" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="3"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
+      <c r="A74" s="9"/>
+      <c r="B74" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="75" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="3"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
+      <c r="A75" s="9"/>
+      <c r="B75" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="76" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="3"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
+      <c r="A76" s="9"/>
+      <c r="B76" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="77" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="3"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
+      <c r="A77" s="9"/>
+      <c r="B77" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="78" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="3"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
+      <c r="A78" s="9"/>
+      <c r="B78" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="79" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="3"/>
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
+      <c r="A79" s="9"/>
+      <c r="B79" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="80" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="3"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
+      <c r="A80" s="9"/>
+      <c r="B80" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="81" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="3"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
+      <c r="A81" s="9"/>
+      <c r="B81" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="82" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="3"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
+      <c r="A82" s="9"/>
+      <c r="B82" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="83" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="3"/>
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
+      <c r="A83" s="9"/>
+      <c r="B83" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="84" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="3"/>
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
+      <c r="A84" s="9"/>
+      <c r="B84" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="85" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="3"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
+      <c r="A85" s="9"/>
+      <c r="B85" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="86" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="3"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
+      <c r="A86" s="9"/>
+      <c r="B86" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="87" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="3"/>
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
+      <c r="A87" s="9"/>
+      <c r="B87" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="88" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="3"/>
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
+      <c r="A88" s="9"/>
+      <c r="B88" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="89" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="3"/>
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
+      <c r="A89" s="9"/>
+      <c r="B89" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="90" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="3"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
+      <c r="A90" s="9"/>
+      <c r="B90" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="91" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="3"/>
-      <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
+      <c r="A91" s="9"/>
+      <c r="B91" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="92" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="3"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
+      <c r="A92" s="9"/>
+      <c r="B92" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="93" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="3"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
+      <c r="A93" s="9"/>
+      <c r="B93" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="94" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="3"/>
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
+      <c r="A94" s="9"/>
+      <c r="B94" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="95" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="3"/>
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
+      <c r="A95" s="9"/>
+      <c r="B95" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="96" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="3"/>
-      <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
+      <c r="A96" s="9"/>
+      <c r="B96" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="97" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="3"/>
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
+      <c r="A97" s="9"/>
+      <c r="B97" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="98" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="3"/>
-      <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
+      <c r="A98" s="9"/>
+      <c r="B98" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="99" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="3"/>
-      <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
+      <c r="A99" s="9"/>
+      <c r="B99" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="100" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="3"/>
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
+      <c r="A100" s="10"/>
+      <c r="B100" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="101" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="3"/>
@@ -1883,11 +2285,12 @@
       <c r="C150" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="A34:A51"/>
     <mergeCell ref="A52:A56"/>
-    <mergeCell ref="A57:A72"/>
+    <mergeCell ref="A57:A71"/>
+    <mergeCell ref="A72:A100"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Finish Create All Submenu sidebar
</commit_message>
<xml_diff>
--- a/List Menu.xlsx
+++ b/List Menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\onlineguide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2188CF-C189-4DE4-9B60-B36FF42857DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DF1026-7DC4-43C3-A53D-9F37213748BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{40BDCF54-5589-495D-8190-883E443269E3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="315">
   <si>
     <t>Menu</t>
   </si>
@@ -323,9 +323,6 @@
     <t>Qualified Transfer of Purchase into Warehouse</t>
   </si>
   <si>
-    <t>qualified_transferofpurchase</t>
-  </si>
-  <si>
     <t>Purchase Receipt Notice</t>
   </si>
   <si>
@@ -569,9 +566,6 @@
     <t>Sales Exit Inspection</t>
   </si>
   <si>
-    <t>sales_exit_inspection</t>
-  </si>
-  <si>
     <t>Maintenance of Stock Notes</t>
   </si>
   <si>
@@ -617,9 +611,6 @@
     <t>Delivery Inspection Details of Sales</t>
   </si>
   <si>
-    <t>delivery_inspection_details_of_sales</t>
-  </si>
-  <si>
     <t>Outbound Planning Confirmation</t>
   </si>
   <si>
@@ -648,6 +639,348 @@
   </si>
   <si>
     <t>material_return_application_production_order</t>
+  </si>
+  <si>
+    <t>Inventory Transfer</t>
+  </si>
+  <si>
+    <t>inventory_transfer</t>
+  </si>
+  <si>
+    <t>Inventory Utilization</t>
+  </si>
+  <si>
+    <t>inventory_utilization</t>
+  </si>
+  <si>
+    <t>Inventory Transfer Scanning Record</t>
+  </si>
+  <si>
+    <t>inventory_transfer_scanning_record</t>
+  </si>
+  <si>
+    <t>Packaging Box Transfer</t>
+  </si>
+  <si>
+    <t>packaging_box_transfer</t>
+  </si>
+  <si>
+    <t>Internal Claim Return</t>
+  </si>
+  <si>
+    <t>internal_claim_return</t>
+  </si>
+  <si>
+    <t>Quality Assurance</t>
+  </si>
+  <si>
+    <t>Types of Sampling Schemes</t>
+  </si>
+  <si>
+    <t>types_of_sampling_schemes</t>
+  </si>
+  <si>
+    <t>Sample Inspection Scheme</t>
+  </si>
+  <si>
+    <t>sample_inspection_scheme</t>
+  </si>
+  <si>
+    <t>Material Allocation for Quality Inspection</t>
+  </si>
+  <si>
+    <t>material_allocation_for_quality_inspection</t>
+  </si>
+  <si>
+    <t>Quality Inspection List</t>
+  </si>
+  <si>
+    <t>quality_inspection_list</t>
+  </si>
+  <si>
+    <t>质检清单项-备品备件</t>
+  </si>
+  <si>
+    <t>Items of Quality Inspection List</t>
+  </si>
+  <si>
+    <t>items_of_quality_inspection_list</t>
+  </si>
+  <si>
+    <t>Statistics of Qualification Rate of Quality Inspection</t>
+  </si>
+  <si>
+    <t>statistics_of_qualification_rate_of_quality_inspection</t>
+  </si>
+  <si>
+    <t>sales_exit_inspection_warehouse</t>
+  </si>
+  <si>
+    <t>sales_exit_inspection_quality</t>
+  </si>
+  <si>
+    <t>delivery_inspection_details_of_sales_warehouse</t>
+  </si>
+  <si>
+    <t>delivery_inspection_details_of_sales_quality</t>
+  </si>
+  <si>
+    <t>qualified_transferofpurchase_warehouse</t>
+  </si>
+  <si>
+    <t>qualified_transferofpurchase_quality</t>
+  </si>
+  <si>
+    <t>Inventory Work</t>
+  </si>
+  <si>
+    <t>Inventory Plan</t>
+  </si>
+  <si>
+    <t>inventory_plan</t>
+  </si>
+  <si>
+    <t>Abnormal Inventory Posting</t>
+  </si>
+  <si>
+    <t>abnormal_inventory_posting</t>
+  </si>
+  <si>
+    <t>Abnormal Inventory Details</t>
+  </si>
+  <si>
+    <t>abnormal_inventory_details</t>
+  </si>
+  <si>
+    <t>Inventory Report</t>
+  </si>
+  <si>
+    <t>inventory_report</t>
+  </si>
+  <si>
+    <t>Inventory Record</t>
+  </si>
+  <si>
+    <t>inventory_record</t>
+  </si>
+  <si>
+    <t>Carry-over Date</t>
+  </si>
+  <si>
+    <t>carry-over_date</t>
+  </si>
+  <si>
+    <t>Calculation of Reservoir Age</t>
+  </si>
+  <si>
+    <t>calculation_of_reservoir_age</t>
+  </si>
+  <si>
+    <t>Monthly Statement of Deposit Age</t>
+  </si>
+  <si>
+    <t>monthly_statement_of_deposit_age</t>
+  </si>
+  <si>
+    <t>certificate_cancellation_monthly</t>
+  </si>
+  <si>
+    <t>Certificate Write-off Record</t>
+  </si>
+  <si>
+    <t>certificate_write-off_record</t>
+  </si>
+  <si>
+    <t>Ending Inventory</t>
+  </si>
+  <si>
+    <t>ending_inventory</t>
+  </si>
+  <si>
+    <t>Monthly Settlement Management</t>
+  </si>
+  <si>
+    <t>Label Management</t>
+  </si>
+  <si>
+    <t>Purchasing Receiving Label Printing</t>
+  </si>
+  <si>
+    <t>purchasing_receiving_label_printing</t>
+  </si>
+  <si>
+    <t>Delivery Label Printing</t>
+  </si>
+  <si>
+    <t>delivery_label_printing</t>
+  </si>
+  <si>
+    <t>Statement Statistics</t>
+  </si>
+  <si>
+    <t>Difference Report of Recoil Material in Line Side Warehouse</t>
+  </si>
+  <si>
+    <t>difference_report_of_recoil_material</t>
+  </si>
+  <si>
+    <t>Line Side Warehouse Direct Feeding Difference Report</t>
+  </si>
+  <si>
+    <t>warehouse_direct_feeding_difference_report</t>
+  </si>
+  <si>
+    <t>Production Consumption Analysis Report</t>
+  </si>
+  <si>
+    <t>production_consumption_analysis_report</t>
+  </si>
+  <si>
+    <t>Safety Inventory Statement</t>
+  </si>
+  <si>
+    <t>safety_inventory_statement</t>
+  </si>
+  <si>
+    <t>Material Inventory Statistics</t>
+  </si>
+  <si>
+    <t>material_inventory_statistics</t>
+  </si>
+  <si>
+    <t>Efficiency Analysis Report</t>
+  </si>
+  <si>
+    <t>efficiency_analysis_report</t>
+  </si>
+  <si>
+    <t>Details of Warehousing</t>
+  </si>
+  <si>
+    <t>details_of_warehousing</t>
+  </si>
+  <si>
+    <t>Details of Deposit</t>
+  </si>
+  <si>
+    <t>details_of_deposit</t>
+  </si>
+  <si>
+    <t>Details of Entry and Exit</t>
+  </si>
+  <si>
+    <t>details_of_entry_and_exit</t>
+  </si>
+  <si>
+    <t>Details of Material Entry and Exit</t>
+  </si>
+  <si>
+    <t>details_of_material_entry_and_exit</t>
+  </si>
+  <si>
+    <t>Document Statement</t>
+  </si>
+  <si>
+    <t>document_statement</t>
+  </si>
+  <si>
+    <t>Inventory Statistics</t>
+  </si>
+  <si>
+    <t>inventory_statistics</t>
+  </si>
+  <si>
+    <t>Inventory Reconciliation</t>
+  </si>
+  <si>
+    <t>inventory_reconciliation</t>
+  </si>
+  <si>
+    <t>Initial Inventory</t>
+  </si>
+  <si>
+    <t>initial_inventory</t>
+  </si>
+  <si>
+    <t>Statistical analysis of sluggish materials</t>
+  </si>
+  <si>
+    <t>statistical_analysis_of_sluggish_materials</t>
+  </si>
+  <si>
+    <t>Outsourcing purchase list execution report</t>
+  </si>
+  <si>
+    <t>outsourcing_purchase_list_execution_report</t>
+  </si>
+  <si>
+    <t>Production validity analysis report</t>
+  </si>
+  <si>
+    <t>production_validity_analysis_report</t>
+  </si>
+  <si>
+    <t>Storage capacity analysis report</t>
+  </si>
+  <si>
+    <t>storage_capacity_analysis_report</t>
+  </si>
+  <si>
+    <t>Packing Information Statement</t>
+  </si>
+  <si>
+    <t>packing_information_statement</t>
+  </si>
+  <si>
+    <t>Internal Acquisition Statement</t>
+  </si>
+  <si>
+    <t>internal_acquisition_statement</t>
+  </si>
+  <si>
+    <t>Details of Internal Receipt and Return</t>
+  </si>
+  <si>
+    <t>details_of_internal_receipt_and_return</t>
+  </si>
+  <si>
+    <t>inventory_attributes_of_finished_products</t>
+  </si>
+  <si>
+    <t>Out-of-stock Report</t>
+  </si>
+  <si>
+    <t>out-of-stock_report</t>
+  </si>
+  <si>
+    <t>Entry and Exit Details</t>
+  </si>
+  <si>
+    <t>entry_and_exit_details</t>
+  </si>
+  <si>
+    <t>Optical Bar Inventory Attribute Statement</t>
+  </si>
+  <si>
+    <t>optical_bar_inventory_attribute_statement</t>
+  </si>
+  <si>
+    <t>Details of Finished Products in and out of Warehouse</t>
+  </si>
+  <si>
+    <t>details_of_finished_products_inout_of_warehouse</t>
+  </si>
+  <si>
+    <t>monthly_statement_of_deposit_age_statistics</t>
+  </si>
+  <si>
+    <t>Sales Order Status Statistics</t>
+  </si>
+  <si>
+    <t>sales_order_status_statistics</t>
+  </si>
+  <si>
+    <t>Inventory Attributes of Finished Products</t>
   </si>
 </sst>
 </file>
@@ -749,30 +1082,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1109,16 +1439,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46758F73-D68C-4007-AE73-B5A0F2E8918A}">
-  <dimension ref="A1:C150"/>
+  <dimension ref="A1:C161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A137" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.453125" customWidth="1"/>
-    <col min="2" max="2" width="43.81640625" customWidth="1"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="50.1796875" customWidth="1"/>
     <col min="3" max="3" width="43.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1134,1163 +1464,1460 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="7"/>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="7"/>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="7"/>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="7"/>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="7"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="7"/>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="7"/>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="7"/>
-      <c r="B18" s="4" t="s">
+      <c r="A18" s="9"/>
+      <c r="B18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="7"/>
-      <c r="B19" s="4" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="7"/>
-      <c r="B20" s="4" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="7"/>
-      <c r="B21" s="4" t="s">
+      <c r="A21" s="9"/>
+      <c r="B21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="7"/>
-      <c r="B22" s="4" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="7"/>
-      <c r="B23" s="4" t="s">
+      <c r="A23" s="9"/>
+      <c r="B23" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="7"/>
-      <c r="B24" s="4" t="s">
+      <c r="A24" s="9"/>
+      <c r="B24" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="7"/>
-      <c r="B25" s="4" t="s">
+      <c r="A25" s="9"/>
+      <c r="B25" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="7"/>
-      <c r="B26" s="4" t="s">
+      <c r="A26" s="9"/>
+      <c r="B26" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="7"/>
-      <c r="B27" s="4" t="s">
+      <c r="A27" s="9"/>
+      <c r="B27" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="7"/>
-      <c r="B28" s="4" t="s">
+      <c r="A28" s="9"/>
+      <c r="B28" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="7"/>
-      <c r="B29" s="4" t="s">
+      <c r="A29" s="9"/>
+      <c r="B29" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="7"/>
-      <c r="B30" s="4" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="7"/>
-      <c r="B31" s="4" t="s">
+      <c r="A31" s="9"/>
+      <c r="B31" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="7"/>
-      <c r="B32" s="4" t="s">
+      <c r="A32" s="9"/>
+      <c r="B32" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="7"/>
-      <c r="B33" s="4" t="s">
+      <c r="A33" s="9"/>
+      <c r="B33" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="9"/>
-      <c r="B35" s="4" t="s">
+      <c r="A35" s="8"/>
+      <c r="B35" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="9"/>
-      <c r="B36" s="4" t="s">
+      <c r="A36" s="8"/>
+      <c r="B36" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="9"/>
-      <c r="B37" s="4" t="s">
+      <c r="A37" s="8"/>
+      <c r="B37" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="9"/>
-      <c r="B38" s="4" t="s">
+      <c r="A38" s="8"/>
+      <c r="B38" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="9"/>
-      <c r="B39" s="5" t="s">
+      <c r="A39" s="8"/>
+      <c r="B39" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="9"/>
-      <c r="B40" s="4" t="s">
+      <c r="A40" s="8"/>
+      <c r="B40" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="9"/>
-      <c r="B41" s="4" t="s">
+      <c r="A41" s="8"/>
+      <c r="B41" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="9"/>
-      <c r="B42" s="4" t="s">
+      <c r="A42" s="8"/>
+      <c r="B42" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="3" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="9"/>
-      <c r="B43" s="4" t="s">
+      <c r="A43" s="8"/>
+      <c r="B43" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="9"/>
-      <c r="B44" s="4" t="s">
+      <c r="A44" s="8"/>
+      <c r="B44" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="8"/>
+      <c r="B45" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="8"/>
+      <c r="B46" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="8"/>
+      <c r="B47" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="8"/>
+      <c r="B48" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="8"/>
+      <c r="B49" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="8"/>
+      <c r="B50" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="8"/>
+      <c r="B51" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="6" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="9"/>
-      <c r="B45" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="9"/>
-      <c r="B46" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="9"/>
-      <c r="B47" s="5" t="s">
+      <c r="B52" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="8"/>
+      <c r="B53" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="8"/>
+      <c r="B54" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="8"/>
+      <c r="B55" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="7"/>
+      <c r="B56" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="8"/>
+      <c r="B58" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="8"/>
+      <c r="B59" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="8"/>
+      <c r="B60" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="8"/>
+      <c r="B61" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="8"/>
+      <c r="B62" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="8"/>
+      <c r="B63" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="8"/>
+      <c r="B64" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="8"/>
+      <c r="B65" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="8"/>
+      <c r="B66" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="8"/>
+      <c r="B67" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="8"/>
+      <c r="B68" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="8"/>
+      <c r="B69" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="8"/>
+      <c r="B70" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="8"/>
+      <c r="B71" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="8"/>
+      <c r="B73" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="8"/>
+      <c r="B74" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="8"/>
+      <c r="B75" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="8"/>
+      <c r="B76" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="8"/>
+      <c r="B77" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="8"/>
+      <c r="B78" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="8"/>
+      <c r="B79" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="8"/>
+      <c r="B80" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="8"/>
+      <c r="B81" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="8"/>
+      <c r="B82" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="8"/>
+      <c r="B83" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="8"/>
+      <c r="B84" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="8"/>
+      <c r="B85" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="8"/>
+      <c r="B86" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="8"/>
+      <c r="B87" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="8"/>
+      <c r="B88" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="8"/>
+      <c r="B89" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="8"/>
+      <c r="B90" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="8"/>
+      <c r="B91" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="8"/>
+      <c r="B92" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="8"/>
+      <c r="B93" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="8"/>
+      <c r="B94" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="8"/>
+      <c r="B95" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="8"/>
+      <c r="B96" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="8"/>
+      <c r="B97" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="8"/>
+      <c r="B98" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="8"/>
+      <c r="B99" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="7"/>
+      <c r="B100" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="8"/>
+      <c r="B102" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="8"/>
+      <c r="B103" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="8"/>
+      <c r="B104" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="7"/>
+      <c r="B105" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A106" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="8"/>
+      <c r="B107" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="8"/>
+      <c r="B108" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="8"/>
+      <c r="B109" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="8"/>
+      <c r="B110" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="8"/>
+      <c r="B111" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="8"/>
+      <c r="B112" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="8"/>
+      <c r="B113" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="8"/>
+      <c r="B114" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="7"/>
+      <c r="B115" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="9"/>
-      <c r="B48" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="9"/>
-      <c r="B49" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="9"/>
-      <c r="B50" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="9"/>
-      <c r="B51" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="9"/>
-      <c r="B53" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="9"/>
-      <c r="B54" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="9"/>
-      <c r="B55" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="10"/>
-      <c r="B56" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="9"/>
-      <c r="B58" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="9"/>
-      <c r="B59" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="9"/>
-      <c r="B60" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="9"/>
-      <c r="B61" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="9"/>
-      <c r="B62" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="9"/>
-      <c r="B63" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="9"/>
-      <c r="B64" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="9"/>
-      <c r="B65" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="9"/>
-      <c r="B66" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="9"/>
-      <c r="B67" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="9"/>
-      <c r="B68" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="9"/>
-      <c r="B69" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="9"/>
-      <c r="B70" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="9"/>
-      <c r="B71" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="9"/>
-      <c r="B73" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="9"/>
-      <c r="B74" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="9"/>
-      <c r="B75" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="9"/>
-      <c r="B76" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="9"/>
-      <c r="B77" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="9"/>
-      <c r="B78" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="9"/>
-      <c r="B79" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="9"/>
-      <c r="B80" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="9"/>
-      <c r="B81" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="9"/>
-      <c r="B82" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="9"/>
-      <c r="B83" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="9"/>
-      <c r="B84" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="9"/>
-      <c r="B85" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="9"/>
-      <c r="B86" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="9"/>
-      <c r="B87" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="9"/>
-      <c r="B88" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="9"/>
-      <c r="B89" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="9"/>
-      <c r="B90" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="9"/>
-      <c r="B91" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="9"/>
-      <c r="B92" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="9"/>
-      <c r="B93" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="9"/>
-      <c r="B94" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="9"/>
-      <c r="B95" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="9"/>
-      <c r="B96" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="9"/>
-      <c r="B97" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="9"/>
-      <c r="B98" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="9"/>
-      <c r="B99" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="10"/>
-      <c r="B100" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="3"/>
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-    </row>
-    <row r="102" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="3"/>
-      <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
-    </row>
-    <row r="103" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="3"/>
-      <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
-    </row>
-    <row r="104" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="3"/>
-      <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
-    </row>
-    <row r="105" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="3"/>
-      <c r="B105" s="2"/>
-      <c r="C105" s="2"/>
-    </row>
-    <row r="106" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="3"/>
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
-    </row>
-    <row r="107" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="3"/>
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
-    </row>
-    <row r="108" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="3"/>
-      <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
-    </row>
-    <row r="109" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="2"/>
-      <c r="B109" s="2"/>
-      <c r="C109" s="2"/>
-    </row>
-    <row r="110" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="2"/>
-      <c r="B110" s="2"/>
-      <c r="C110" s="2"/>
-    </row>
-    <row r="111" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="2"/>
-      <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
-    </row>
-    <row r="112" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="2"/>
-      <c r="B112" s="2"/>
-      <c r="C112" s="2"/>
-    </row>
-    <row r="113" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="2"/>
-      <c r="B113" s="2"/>
-      <c r="C113" s="2"/>
-    </row>
-    <row r="114" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="2"/>
-      <c r="B114" s="2"/>
-      <c r="C114" s="2"/>
-    </row>
-    <row r="115" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="2"/>
-      <c r="B115" s="2"/>
-      <c r="C115" s="2"/>
+      <c r="C115" s="3" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="116" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="2"/>
-      <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
+      <c r="A116" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="117" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="2"/>
-      <c r="B117" s="2"/>
-      <c r="C117" s="2"/>
+      <c r="A117" s="8"/>
+      <c r="B117" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="118" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="2"/>
-      <c r="B118" s="2"/>
-      <c r="C118" s="2"/>
+      <c r="A118" s="8"/>
+      <c r="B118" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="119" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="2"/>
-      <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
+      <c r="A119" s="8"/>
+      <c r="B119" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="120" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="2"/>
-      <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
+      <c r="A120" s="7"/>
+      <c r="B120" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="121" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="2"/>
-      <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
+      <c r="A121" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="122" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="2"/>
-      <c r="B122" s="2"/>
-      <c r="C122" s="2"/>
+      <c r="A122" s="8"/>
+      <c r="B122" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="123" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="2"/>
-      <c r="B123" s="2"/>
-      <c r="C123" s="2"/>
+      <c r="A123" s="8"/>
+      <c r="B123" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="124" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="2"/>
-      <c r="B124" s="2"/>
-      <c r="C124" s="2"/>
+      <c r="A124" s="8"/>
+      <c r="B124" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="125" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="2"/>
-      <c r="B125" s="2"/>
-      <c r="C125" s="2"/>
+      <c r="A125" s="8"/>
+      <c r="B125" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="126" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="2"/>
-      <c r="B126" s="2"/>
-      <c r="C126" s="2"/>
+      <c r="A126" s="7"/>
+      <c r="B126" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="127" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A127" s="2"/>
-      <c r="B127" s="2"/>
-      <c r="C127" s="2"/>
+      <c r="A127" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="128" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="2"/>
-      <c r="B128" s="2"/>
-      <c r="C128" s="2"/>
+      <c r="A128" s="7"/>
+      <c r="B128" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="129" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="2"/>
-      <c r="B129" s="2"/>
-      <c r="C129" s="2"/>
+      <c r="A129" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="130" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="2"/>
-      <c r="B130" s="2"/>
-      <c r="C130" s="2"/>
+      <c r="A130" s="8"/>
+      <c r="B130" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="131" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="2"/>
-      <c r="B131" s="2"/>
-      <c r="C131" s="2"/>
+      <c r="A131" s="8"/>
+      <c r="B131" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="132" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A132" s="2"/>
-      <c r="B132" s="2"/>
-      <c r="C132" s="2"/>
+      <c r="A132" s="8"/>
+      <c r="B132" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="133" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="2"/>
-      <c r="B133" s="2"/>
-      <c r="C133" s="2"/>
+      <c r="A133" s="8"/>
+      <c r="B133" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="134" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="2"/>
-      <c r="B134" s="2"/>
-      <c r="C134" s="2"/>
+      <c r="A134" s="8"/>
+      <c r="B134" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="135" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="2"/>
-      <c r="B135" s="2"/>
-      <c r="C135" s="2"/>
+      <c r="A135" s="8"/>
+      <c r="B135" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="136" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="2"/>
-      <c r="B136" s="2"/>
-      <c r="C136" s="2"/>
+      <c r="A136" s="8"/>
+      <c r="B136" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="137" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="2"/>
-      <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
+      <c r="A137" s="8"/>
+      <c r="B137" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="138" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="2"/>
-      <c r="B138" s="2"/>
-      <c r="C138" s="2"/>
+      <c r="A138" s="8"/>
+      <c r="B138" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="139" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="2"/>
-      <c r="B139" s="2"/>
-      <c r="C139" s="2"/>
+      <c r="A139" s="8"/>
+      <c r="B139" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="140" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="2"/>
-      <c r="B140" s="2"/>
-      <c r="C140" s="2"/>
+      <c r="A140" s="8"/>
+      <c r="B140" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="141" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="2"/>
-      <c r="B141" s="2"/>
-      <c r="C141" s="2"/>
+      <c r="A141" s="8"/>
+      <c r="B141" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="142" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="2"/>
-      <c r="B142" s="2"/>
-      <c r="C142" s="2"/>
+      <c r="A142" s="8"/>
+      <c r="B142" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="143" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A143" s="2"/>
-      <c r="B143" s="2"/>
-      <c r="C143" s="2"/>
+      <c r="A143" s="8"/>
+      <c r="B143" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="144" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="2"/>
-      <c r="B144" s="2"/>
-      <c r="C144" s="2"/>
+      <c r="A144" s="8"/>
+      <c r="B144" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="145" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="2"/>
-      <c r="B145" s="2"/>
-      <c r="C145" s="2"/>
+      <c r="A145" s="8"/>
+      <c r="B145" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="146" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="2"/>
-      <c r="B146" s="2"/>
-      <c r="C146" s="2"/>
+      <c r="A146" s="8"/>
+      <c r="B146" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="147" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="2"/>
-      <c r="B147" s="2"/>
-      <c r="C147" s="2"/>
+      <c r="A147" s="8"/>
+      <c r="B147" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="148" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A148" s="2"/>
-      <c r="B148" s="2"/>
-      <c r="C148" s="2"/>
+      <c r="A148" s="8"/>
+      <c r="B148" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="149" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A149" s="2"/>
-      <c r="B149" s="2"/>
-      <c r="C149" s="2"/>
+      <c r="A149" s="8"/>
+      <c r="B149" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="150" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A150" s="2"/>
-      <c r="B150" s="2"/>
-      <c r="C150" s="2"/>
+      <c r="A150" s="8"/>
+      <c r="B150" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A151" s="8"/>
+      <c r="B151" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A152" s="8"/>
+      <c r="B152" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A153" s="8"/>
+      <c r="B153" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A154" s="8"/>
+      <c r="B154" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A155" s="8"/>
+      <c r="B155" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A156" s="7"/>
+      <c r="B156" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A157" s="2"/>
+      <c r="B157" s="2"/>
+      <c r="C157" s="2"/>
+    </row>
+    <row r="158" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A158" s="2"/>
+      <c r="B158" s="2"/>
+      <c r="C158" s="2"/>
+    </row>
+    <row r="159" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A159" s="2"/>
+      <c r="B159" s="2"/>
+      <c r="C159" s="2"/>
+    </row>
+    <row r="160" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A160" s="2"/>
+      <c r="B160" s="2"/>
+      <c r="C160" s="2"/>
+    </row>
+    <row r="161" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A161" s="2"/>
+      <c r="B161" s="2"/>
+      <c r="C161" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="11">
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="A34:A51"/>
     <mergeCell ref="A52:A56"/>
     <mergeCell ref="A57:A71"/>
     <mergeCell ref="A72:A100"/>
+    <mergeCell ref="A127:A128"/>
+    <mergeCell ref="A129:A156"/>
+    <mergeCell ref="A101:A105"/>
+    <mergeCell ref="A106:A115"/>
+    <mergeCell ref="A116:A120"/>
+    <mergeCell ref="A121:A126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>